<commit_message>
Se agrego el cronograma del projecto
</commit_message>
<xml_diff>
--- a/Desarrollo/RP/Gestion/RP-CP.xlsx
+++ b/Desarrollo/RP/Gestion/RP-CP.xlsx
@@ -1397,7 +1397,7 @@
         <v>45404.0</v>
       </c>
       <c r="J18" s="32">
-        <v>45407.0</v>
+        <v>45410.0</v>
       </c>
       <c r="K18" s="45">
         <v>1.0</v>
@@ -1424,7 +1424,7 @@
         <v>45404.0</v>
       </c>
       <c r="J19" s="32">
-        <v>45407.0</v>
+        <v>45410.0</v>
       </c>
       <c r="K19" s="45">
         <v>1.0</v>
@@ -1451,7 +1451,7 @@
         <v>45404.0</v>
       </c>
       <c r="J20" s="32">
-        <v>45407.0</v>
+        <v>45410.0</v>
       </c>
       <c r="K20" s="45">
         <v>1.0</v>
@@ -1478,7 +1478,7 @@
         <v>45404.0</v>
       </c>
       <c r="J21" s="32">
-        <v>45407.0</v>
+        <v>45410.0</v>
       </c>
       <c r="K21" s="45">
         <v>1.0</v>
@@ -1505,7 +1505,7 @@
         <v>45404.0</v>
       </c>
       <c r="J22" s="32">
-        <v>45407.0</v>
+        <v>45410.0</v>
       </c>
       <c r="K22" s="45">
         <v>1.0</v>
@@ -1532,7 +1532,7 @@
         <v>45404.0</v>
       </c>
       <c r="J23" s="32">
-        <v>45407.0</v>
+        <v>45410.0</v>
       </c>
       <c r="K23" s="45">
         <v>1.0</v>
@@ -1559,7 +1559,7 @@
         <v>45404.0</v>
       </c>
       <c r="J24" s="32">
-        <v>45407.0</v>
+        <v>45410.0</v>
       </c>
       <c r="K24" s="45">
         <v>1.0</v>
@@ -1586,7 +1586,7 @@
         <v>45404.0</v>
       </c>
       <c r="J25" s="32">
-        <v>45407.0</v>
+        <v>45410.0</v>
       </c>
       <c r="K25" s="45">
         <v>1.0</v>
@@ -1616,7 +1616,7 @@
         <v>45404</v>
       </c>
       <c r="J26" s="32">
-        <v>45407.0</v>
+        <v>45410.0</v>
       </c>
       <c r="K26" s="45">
         <v>1.0</v>
@@ -1639,11 +1639,11 @@
       <c r="H27" s="31"/>
       <c r="I27" s="38">
         <f>J26</f>
-        <v>45407</v>
+        <v>45410</v>
       </c>
       <c r="J27" s="38">
         <f>I27+5</f>
-        <v>45412</v>
+        <v>45415</v>
       </c>
       <c r="K27" s="52">
         <v>0.0</v>
@@ -1670,11 +1670,11 @@
       </c>
       <c r="I28" s="38">
         <f>J26+1</f>
-        <v>45408</v>
+        <v>45411</v>
       </c>
       <c r="J28" s="38">
         <f t="shared" ref="J28:J29" si="1">I28+3</f>
-        <v>45411</v>
+        <v>45414</v>
       </c>
       <c r="K28" s="52">
         <v>0.0</v>
@@ -1701,11 +1701,11 @@
       </c>
       <c r="I29" s="38">
         <f>J26+1</f>
-        <v>45408</v>
+        <v>45411</v>
       </c>
       <c r="J29" s="38">
         <f t="shared" si="1"/>
-        <v>45411</v>
+        <v>45414</v>
       </c>
       <c r="K29" s="52">
         <v>0.0</v>
@@ -1728,11 +1728,11 @@
       <c r="H30" s="31"/>
       <c r="I30" s="38">
         <f>J26+1</f>
-        <v>45408</v>
+        <v>45411</v>
       </c>
       <c r="J30" s="38">
         <f>I30+4</f>
-        <v>45412</v>
+        <v>45415</v>
       </c>
       <c r="K30" s="52">
         <v>0.0</v>
@@ -1759,11 +1759,11 @@
       </c>
       <c r="I31" s="38">
         <f>J30+3</f>
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="J31" s="38">
         <f>I31+3</f>
-        <v>45418</v>
+        <v>45421</v>
       </c>
       <c r="K31" s="52">
         <v>0.0</v>
@@ -1788,11 +1788,11 @@
       <c r="H32" s="31"/>
       <c r="I32" s="38">
         <f t="shared" ref="I32:I33" si="2">J31</f>
-        <v>45418</v>
+        <v>45421</v>
       </c>
       <c r="J32" s="38">
         <f t="shared" ref="J32:J33" si="3">I32</f>
-        <v>45418</v>
+        <v>45421</v>
       </c>
       <c r="K32" s="52">
         <v>0.0</v>
@@ -1817,11 +1817,11 @@
       <c r="H33" s="31"/>
       <c r="I33" s="38">
         <f t="shared" si="2"/>
-        <v>45418</v>
+        <v>45421</v>
       </c>
       <c r="J33" s="38">
         <f t="shared" si="3"/>
-        <v>45418</v>
+        <v>45421</v>
       </c>
       <c r="K33" s="52">
         <v>0.0</v>
@@ -1867,11 +1867,11 @@
       </c>
       <c r="I35" s="38">
         <f>J33+1</f>
-        <v>45419</v>
+        <v>45422</v>
       </c>
       <c r="J35" s="38">
         <f>I35+6</f>
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="K35" s="52">
         <v>0.0</v>
@@ -1900,11 +1900,11 @@
       </c>
       <c r="I36" s="38">
         <f>J33+1</f>
-        <v>45419</v>
+        <v>45422</v>
       </c>
       <c r="J36" s="38">
         <f>I36+10</f>
-        <v>45429</v>
+        <v>45432</v>
       </c>
       <c r="K36" s="52">
         <v>0.0</v>
@@ -1931,11 +1931,11 @@
       <c r="H37" s="31"/>
       <c r="I37" s="38">
         <f>I35+3</f>
-        <v>45422</v>
+        <v>45425</v>
       </c>
       <c r="J37" s="38">
         <f>I37+4</f>
-        <v>45426</v>
+        <v>45429</v>
       </c>
       <c r="K37" s="52">
         <v>0.0</v>
@@ -1962,11 +1962,11 @@
       <c r="H38" s="30"/>
       <c r="I38" s="38">
         <f>J33+1</f>
-        <v>45419</v>
+        <v>45422</v>
       </c>
       <c r="J38" s="38">
-        <f>I38+8</f>
-        <v>45427</v>
+        <f>I38+4</f>
+        <v>45426</v>
       </c>
       <c r="K38" s="52">
         <v>0.0</v>
@@ -1993,11 +1993,11 @@
       <c r="H39" s="31"/>
       <c r="I39" s="38">
         <f t="shared" ref="I39:I40" si="4">J38</f>
-        <v>45427</v>
+        <v>45426</v>
       </c>
       <c r="J39" s="38">
         <f>I39+5</f>
-        <v>45432</v>
+        <v>45431</v>
       </c>
       <c r="K39" s="52">
         <v>0.0</v>
@@ -2024,11 +2024,11 @@
       <c r="H40" s="31"/>
       <c r="I40" s="38">
         <f t="shared" si="4"/>
-        <v>45432</v>
+        <v>45431</v>
       </c>
       <c r="J40" s="38">
         <f>I40+7</f>
-        <v>45439</v>
+        <v>45438</v>
       </c>
       <c r="K40" s="52">
         <v>0.0</v>
@@ -2055,11 +2055,11 @@
       <c r="H41" s="30"/>
       <c r="I41" s="38">
         <f>I40+3</f>
-        <v>45435</v>
+        <v>45434</v>
       </c>
       <c r="J41" s="38">
         <f>I41+6</f>
-        <v>45441</v>
+        <v>45440</v>
       </c>
       <c r="K41" s="52">
         <v>0.0</v>
@@ -2088,11 +2088,11 @@
       </c>
       <c r="I42" s="38">
         <f>J41+1</f>
-        <v>45442</v>
+        <v>45441</v>
       </c>
       <c r="J42" s="38">
         <f>I42+4</f>
-        <v>45446</v>
+        <v>45445</v>
       </c>
       <c r="K42" s="52">
         <v>0.0</v>
@@ -2119,11 +2119,11 @@
       <c r="H43" s="31"/>
       <c r="I43" s="38">
         <f>J41</f>
-        <v>45441</v>
+        <v>45440</v>
       </c>
       <c r="J43" s="38">
         <f t="shared" ref="J43:J44" si="5">I43+2</f>
-        <v>45443</v>
+        <v>45442</v>
       </c>
       <c r="K43" s="52">
         <v>0.0</v>
@@ -2148,11 +2148,11 @@
       <c r="H44" s="31"/>
       <c r="I44" s="38">
         <f t="shared" ref="I44:I45" si="6">J43+1</f>
-        <v>45444</v>
+        <v>45443</v>
       </c>
       <c r="J44" s="38">
         <f t="shared" si="5"/>
-        <v>45446</v>
+        <v>45445</v>
       </c>
       <c r="K44" s="52">
         <v>0.0</v>
@@ -2177,11 +2177,11 @@
       <c r="H45" s="59"/>
       <c r="I45" s="60">
         <f t="shared" si="6"/>
-        <v>45447</v>
+        <v>45446</v>
       </c>
       <c r="J45" s="60">
         <f>I45</f>
-        <v>45447</v>
+        <v>45446</v>
       </c>
       <c r="K45" s="52">
         <v>0.0</v>
@@ -2221,11 +2221,11 @@
       <c r="H47" s="61"/>
       <c r="I47" s="62">
         <f>J45+1</f>
-        <v>45448</v>
+        <v>45447</v>
       </c>
       <c r="J47" s="62">
         <f t="shared" ref="J47:J51" si="7">I47</f>
-        <v>45448</v>
+        <v>45447</v>
       </c>
       <c r="K47" s="52">
         <v>0.0</v>
@@ -2250,11 +2250,11 @@
       <c r="H48" s="61"/>
       <c r="I48" s="62">
         <f t="shared" ref="I48:I51" si="8">J47+1</f>
-        <v>45449</v>
+        <v>45448</v>
       </c>
       <c r="J48" s="62">
         <f t="shared" si="7"/>
-        <v>45449</v>
+        <v>45448</v>
       </c>
       <c r="K48" s="52">
         <v>0.0</v>
@@ -2277,11 +2277,11 @@
       <c r="H49" s="61"/>
       <c r="I49" s="62">
         <f t="shared" si="8"/>
-        <v>45450</v>
+        <v>45449</v>
       </c>
       <c r="J49" s="62">
         <f t="shared" si="7"/>
-        <v>45450</v>
+        <v>45449</v>
       </c>
       <c r="K49" s="52">
         <v>0.0</v>
@@ -2306,11 +2306,11 @@
       <c r="H50" s="61"/>
       <c r="I50" s="62">
         <f t="shared" si="8"/>
-        <v>45451</v>
+        <v>45450</v>
       </c>
       <c r="J50" s="62">
         <f t="shared" si="7"/>
-        <v>45451</v>
+        <v>45450</v>
       </c>
       <c r="K50" s="52">
         <v>0.0</v>
@@ -2335,11 +2335,11 @@
       <c r="H51" s="61"/>
       <c r="I51" s="62">
         <f t="shared" si="8"/>
-        <v>45452</v>
+        <v>45451</v>
       </c>
       <c r="J51" s="62">
         <f t="shared" si="7"/>
-        <v>45452</v>
+        <v>45451</v>
       </c>
       <c r="K51" s="52">
         <v>0.0</v>
@@ -2368,11 +2368,11 @@
       </c>
       <c r="I52" s="38">
         <f>J49+1</f>
-        <v>45451</v>
+        <v>45450</v>
       </c>
       <c r="J52" s="38">
         <f>I52+3</f>
-        <v>45454</v>
+        <v>45453</v>
       </c>
       <c r="K52" s="52">
         <v>0.0</v>
@@ -2401,11 +2401,11 @@
       </c>
       <c r="I53" s="62">
         <f>J50</f>
-        <v>45451</v>
+        <v>45450</v>
       </c>
       <c r="J53" s="62">
         <f t="shared" ref="J53:J54" si="9">I53+2</f>
-        <v>45453</v>
+        <v>45452</v>
       </c>
       <c r="K53" s="52">
         <v>0.0</v>
@@ -2430,11 +2430,11 @@
       <c r="H54" s="61"/>
       <c r="I54" s="62">
         <f t="shared" ref="I54:I55" si="10">J53+1</f>
-        <v>45454</v>
+        <v>45453</v>
       </c>
       <c r="J54" s="62">
         <f t="shared" si="9"/>
-        <v>45456</v>
+        <v>45455</v>
       </c>
       <c r="K54" s="52">
         <v>0.0</v>
@@ -2459,11 +2459,11 @@
       <c r="H55" s="31"/>
       <c r="I55" s="38">
         <f t="shared" si="10"/>
-        <v>45457</v>
+        <v>45456</v>
       </c>
       <c r="J55" s="38">
         <f>I55</f>
-        <v>45457</v>
+        <v>45456</v>
       </c>
       <c r="K55" s="52">
         <v>0.0</v>
@@ -2509,11 +2509,11 @@
       </c>
       <c r="I57" s="38">
         <f>J55</f>
-        <v>45457</v>
+        <v>45456</v>
       </c>
       <c r="J57" s="38">
         <f t="shared" ref="J57:J58" si="11">I57+2</f>
-        <v>45459</v>
+        <v>45458</v>
       </c>
       <c r="K57" s="52">
         <v>0.0</v>
@@ -2542,11 +2542,11 @@
       </c>
       <c r="I58" s="38">
         <f>J55</f>
-        <v>45457</v>
+        <v>45456</v>
       </c>
       <c r="J58" s="38">
         <f t="shared" si="11"/>
-        <v>45459</v>
+        <v>45458</v>
       </c>
       <c r="K58" s="52">
         <v>0.0</v>
@@ -2571,11 +2571,11 @@
       <c r="H59" s="31"/>
       <c r="I59" s="38">
         <f t="shared" ref="I59:I60" si="12">J58+1</f>
-        <v>45460</v>
+        <v>45459</v>
       </c>
       <c r="J59" s="38">
         <f>I59+1</f>
-        <v>45461</v>
+        <v>45460</v>
       </c>
       <c r="K59" s="52">
         <v>0.0</v>
@@ -2600,11 +2600,11 @@
       <c r="H60" s="31"/>
       <c r="I60" s="38">
         <f t="shared" si="12"/>
-        <v>45462</v>
+        <v>45461</v>
       </c>
       <c r="J60" s="38">
         <f>I60+3</f>
-        <v>45465</v>
+        <v>45464</v>
       </c>
       <c r="K60" s="52">
         <v>0.0</v>
@@ -2632,7 +2632,7 @@
       </c>
       <c r="D63" s="65">
         <f>J33</f>
-        <v>45418</v>
+        <v>45421</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="D64" s="66">
         <f>J45</f>
-        <v>45447</v>
+        <v>45446</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="D65" s="66">
         <f>J55</f>
-        <v>45457</v>
+        <v>45456</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Se actualizo el avance en el cronograma, RP-DEBD.docx y RP-DDA , en un 80% y 33% respectivamente
</commit_message>
<xml_diff>
--- a/Desarrollo/RP/Gestion/RP-CP.xlsx
+++ b/Desarrollo/RP/Gestion/RP-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amce\Desktop\Reporta-PE\Desarrollo\RP\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F956F4BC-9580-42B7-8287-9D27496CF52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D586B09-8F65-4C87-B75A-CA8C97AD0634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -811,11 +811,20 @@
     <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -826,15 +835,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1053,7 +1053,7 @@
   <dimension ref="A1:K1005"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1071,18 +1071,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
     </row>
     <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
@@ -1098,10 +1098,10 @@
       <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="39"/>
+      <c r="H3" s="40"/>
       <c r="I3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1116,10 +1116,10 @@
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="39"/>
+      <c r="H4" s="40"/>
       <c r="I4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1134,10 +1134,10 @@
       <c r="F5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="39"/>
+      <c r="H5" s="40"/>
       <c r="I5" s="5" t="s">
         <v>14</v>
       </c>
@@ -1152,10 +1152,10 @@
       <c r="F6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="50" t="s">
+      <c r="G6" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="39"/>
+      <c r="H6" s="40"/>
       <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
@@ -1188,10 +1188,10 @@
       <c r="F8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="44"/>
+      <c r="H8" s="49"/>
       <c r="I8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1202,10 +1202,10 @@
       <c r="F9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="44"/>
+      <c r="H9" s="49"/>
       <c r="I9" s="5" t="s">
         <v>30</v>
       </c>
@@ -1216,20 +1216,20 @@
       <c r="F10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="39"/>
+      <c r="H10" s="40"/>
       <c r="I10" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="39"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="40"/>
     </row>
     <row r="13" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
@@ -1267,7 +1267,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="45" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="17" t="s">
@@ -1295,7 +1295,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="17" t="s">
         <v>49</v>
       </c>
@@ -1324,7 +1324,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="17" t="s">
         <v>53</v>
       </c>
@@ -1351,7 +1351,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="41"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="17" t="s">
         <v>57</v>
       </c>
@@ -1379,7 +1379,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="23" t="s">
         <v>61</v>
       </c>
@@ -1406,7 +1406,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="41"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="23" t="s">
         <v>64</v>
       </c>
@@ -1435,7 +1435,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="41"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="23" t="s">
         <v>69</v>
       </c>
@@ -1462,7 +1462,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="41"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="23" t="s">
         <v>72</v>
       </c>
@@ -1489,7 +1489,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="41"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="23" t="s">
         <v>76</v>
       </c>
@@ -1516,7 +1516,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="41"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="23" t="s">
         <v>79</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="41"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="23" t="s">
         <v>83</v>
       </c>
@@ -1570,7 +1570,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="41"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="23" t="s">
         <v>87</v>
       </c>
@@ -1597,7 +1597,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="41"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="23" t="s">
         <v>90</v>
       </c>
@@ -1624,7 +1624,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="41"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="17" t="s">
         <v>94</v>
       </c>
@@ -1652,7 +1652,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="41"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="17" t="s">
         <v>95</v>
       </c>
@@ -1681,7 +1681,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="41"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="17" t="s">
         <v>96</v>
       </c>
@@ -1714,7 +1714,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="41"/>
+      <c r="A30" s="46"/>
       <c r="B30" s="17" t="s">
         <v>99</v>
       </c>
@@ -1747,7 +1747,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="41"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="17" t="s">
         <v>102</v>
       </c>
@@ -1776,7 +1776,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="41"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="17" t="s">
         <v>105</v>
       </c>
@@ -1809,7 +1809,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="41"/>
+      <c r="A33" s="46"/>
       <c r="B33" s="17" t="s">
         <v>108</v>
       </c>
@@ -1838,7 +1838,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="42"/>
+      <c r="A34" s="47"/>
       <c r="B34" s="28" t="s">
         <v>109</v>
       </c>
@@ -1867,22 +1867,22 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="39"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="40"/>
       <c r="I35" s="30"/>
       <c r="J35" s="30"/>
       <c r="K35" s="30"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="45" t="s">
         <v>112</v>
       </c>
       <c r="B36" s="17" t="s">
@@ -1913,7 +1913,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="41"/>
+      <c r="A37" s="46"/>
       <c r="B37" s="17" t="s">
         <v>115</v>
       </c>
@@ -1942,7 +1942,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="41"/>
+      <c r="A38" s="46"/>
       <c r="B38" s="17" t="s">
         <v>116</v>
       </c>
@@ -1971,7 +1971,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="41"/>
+      <c r="A39" s="46"/>
       <c r="B39" s="17" t="s">
         <v>117</v>
       </c>
@@ -2000,7 +2000,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="41"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="17" t="s">
         <v>118</v>
       </c>
@@ -2029,7 +2029,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="41"/>
+      <c r="A41" s="46"/>
       <c r="B41" s="17" t="s">
         <v>119</v>
       </c>
@@ -2058,7 +2058,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="41"/>
+      <c r="A42" s="46"/>
       <c r="B42" s="17" t="s">
         <v>120</v>
       </c>
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="41"/>
+      <c r="A43" s="46"/>
       <c r="B43" s="17" t="s">
         <v>121</v>
       </c>
@@ -2116,7 +2116,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="41"/>
+      <c r="A44" s="46"/>
       <c r="B44" s="17" t="s">
         <v>122</v>
       </c>
@@ -2145,7 +2145,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="42"/>
+      <c r="A45" s="47"/>
       <c r="B45" s="28" t="s">
         <v>123</v>
       </c>
@@ -2174,22 +2174,22 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="37" t="s">
+      <c r="A46" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="39"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="40"/>
       <c r="I46" s="30"/>
       <c r="J46" s="30"/>
       <c r="K46" s="30"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="40" t="s">
+      <c r="A47" s="45" t="s">
         <v>126</v>
       </c>
       <c r="B47" s="17" t="s">
@@ -2222,7 +2222,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="41"/>
+      <c r="A48" s="46"/>
       <c r="B48" s="17" t="s">
         <v>131</v>
       </c>
@@ -2253,7 +2253,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="41"/>
+      <c r="A49" s="46"/>
       <c r="B49" s="33" t="s">
         <v>132</v>
       </c>
@@ -2286,7 +2286,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="41"/>
+      <c r="A50" s="46"/>
       <c r="B50" s="33" t="s">
         <v>133</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="41"/>
+      <c r="A51" s="46"/>
       <c r="B51" s="17" t="s">
         <v>134</v>
       </c>
@@ -2346,7 +2346,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="42"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="28" t="s">
         <v>135</v>
       </c>
@@ -2375,22 +2375,22 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="37" t="s">
+      <c r="A53" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="39"/>
+      <c r="B53" s="44"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
+      <c r="H53" s="40"/>
       <c r="I53" s="30"/>
       <c r="J53" s="30"/>
       <c r="K53" s="30"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="40" t="s">
+      <c r="A54" s="45" t="s">
         <v>138</v>
       </c>
       <c r="B54" s="17" t="s">
@@ -2425,7 +2425,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="41"/>
+      <c r="A55" s="46"/>
       <c r="B55" s="17" t="s">
         <v>142</v>
       </c>
@@ -2458,7 +2458,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="41"/>
+      <c r="A56" s="46"/>
       <c r="B56" s="17" t="s">
         <v>143</v>
       </c>
@@ -2487,7 +2487,7 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="42"/>
+      <c r="A57" s="47"/>
       <c r="B57" s="17" t="s">
         <v>144</v>
       </c>
@@ -2516,16 +2516,16 @@
       </c>
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="37" t="s">
+      <c r="A58" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="B58" s="38"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="38"/>
-      <c r="H58" s="39"/>
+      <c r="B58" s="44"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="44"/>
+      <c r="H58" s="40"/>
       <c r="I58" s="30"/>
       <c r="J58" s="30"/>
       <c r="K58" s="30"/>
@@ -3511,11 +3511,6 @@
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
     <mergeCell ref="A58:H58"/>
     <mergeCell ref="A47:A52"/>
     <mergeCell ref="A36:A45"/>
@@ -3528,6 +3523,11 @@
     <mergeCell ref="A35:H35"/>
     <mergeCell ref="A46:H46"/>
     <mergeCell ref="A53:H53"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F14 F15:G15 F16:F28 F29:H30 F31 F32:H32 F33:F34 F36:F45 F47:G48 F49:H49 F50:G50 F51:F52 F54:H55 F56:F57" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Se actualizo el avance en el cronograma RP-CP.xlsx, (RP-DEBD.docx Y RP-DDA.docx en un 80% y 33% respectivamente)
</commit_message>
<xml_diff>
--- a/Desarrollo/RP/Gestion/RP-CP.xlsx
+++ b/Desarrollo/RP/Gestion/RP-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amce\Desktop\Reporta-PE\Desarrollo\RP\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D586B09-8F65-4C87-B75A-CA8C97AD0634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F30633-F65D-46E8-BC8F-3B56166D7DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -811,20 +811,11 @@
     <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -835,6 +826,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1071,18 +1071,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
     </row>
     <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
@@ -1098,10 +1098,10 @@
       <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="40"/>
+      <c r="H3" s="39"/>
       <c r="I3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1116,10 +1116,10 @@
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="40"/>
+      <c r="H4" s="39"/>
       <c r="I4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1134,10 +1134,10 @@
       <c r="F5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="40"/>
+      <c r="H5" s="39"/>
       <c r="I5" s="5" t="s">
         <v>14</v>
       </c>
@@ -1152,10 +1152,10 @@
       <c r="F6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="40"/>
+      <c r="H6" s="39"/>
       <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
@@ -1188,10 +1188,10 @@
       <c r="F8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="48" t="s">
+      <c r="G8" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="49"/>
+      <c r="H8" s="44"/>
       <c r="I8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1202,10 +1202,10 @@
       <c r="F9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="50" t="s">
+      <c r="G9" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="49"/>
+      <c r="H9" s="44"/>
       <c r="I9" s="5" t="s">
         <v>30</v>
       </c>
@@ -1216,20 +1216,20 @@
       <c r="F10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="40"/>
+      <c r="H10" s="39"/>
       <c r="I10" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="F12" s="43" t="s">
+      <c r="F12" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="44"/>
-      <c r="H12" s="40"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="39"/>
     </row>
     <row r="13" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
@@ -1267,7 +1267,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="40" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="17" t="s">
@@ -1295,7 +1295,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="46"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="17" t="s">
         <v>49</v>
       </c>
@@ -1324,7 +1324,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="17" t="s">
         <v>53</v>
       </c>
@@ -1351,7 +1351,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="46"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="17" t="s">
         <v>57</v>
       </c>
@@ -1379,7 +1379,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="46"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="23" t="s">
         <v>61</v>
       </c>
@@ -1406,7 +1406,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="46"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="23" t="s">
         <v>64</v>
       </c>
@@ -1435,7 +1435,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="46"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="23" t="s">
         <v>69</v>
       </c>
@@ -1462,7 +1462,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="46"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="23" t="s">
         <v>72</v>
       </c>
@@ -1489,7 +1489,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="46"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="23" t="s">
         <v>76</v>
       </c>
@@ -1516,7 +1516,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="46"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="23" t="s">
         <v>79</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="46"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="23" t="s">
         <v>83</v>
       </c>
@@ -1570,7 +1570,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="46"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="23" t="s">
         <v>87</v>
       </c>
@@ -1597,7 +1597,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="46"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="23" t="s">
         <v>90</v>
       </c>
@@ -1624,7 +1624,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="46"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="17" t="s">
         <v>94</v>
       </c>
@@ -1652,7 +1652,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="46"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="17" t="s">
         <v>95</v>
       </c>
@@ -1681,7 +1681,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="46"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="17" t="s">
         <v>96</v>
       </c>
@@ -1714,7 +1714,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="46"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="17" t="s">
         <v>99</v>
       </c>
@@ -1747,7 +1747,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="46"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="17" t="s">
         <v>102</v>
       </c>
@@ -1776,7 +1776,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="46"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="17" t="s">
         <v>105</v>
       </c>
@@ -1809,7 +1809,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="46"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="17" t="s">
         <v>108</v>
       </c>
@@ -1838,7 +1838,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="47"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="28" t="s">
         <v>109</v>
       </c>
@@ -1867,22 +1867,22 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="40"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="39"/>
       <c r="I35" s="30"/>
       <c r="J35" s="30"/>
       <c r="K35" s="30"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="40" t="s">
         <v>112</v>
       </c>
       <c r="B36" s="17" t="s">
@@ -1913,7 +1913,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="46"/>
+      <c r="A37" s="41"/>
       <c r="B37" s="17" t="s">
         <v>115</v>
       </c>
@@ -1942,7 +1942,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="46"/>
+      <c r="A38" s="41"/>
       <c r="B38" s="17" t="s">
         <v>116</v>
       </c>
@@ -1971,7 +1971,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="46"/>
+      <c r="A39" s="41"/>
       <c r="B39" s="17" t="s">
         <v>117</v>
       </c>
@@ -2000,7 +2000,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="46"/>
+      <c r="A40" s="41"/>
       <c r="B40" s="17" t="s">
         <v>118</v>
       </c>
@@ -2029,7 +2029,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="46"/>
+      <c r="A41" s="41"/>
       <c r="B41" s="17" t="s">
         <v>119</v>
       </c>
@@ -2058,7 +2058,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="46"/>
+      <c r="A42" s="41"/>
       <c r="B42" s="17" t="s">
         <v>120</v>
       </c>
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="46"/>
+      <c r="A43" s="41"/>
       <c r="B43" s="17" t="s">
         <v>121</v>
       </c>
@@ -2116,7 +2116,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="46"/>
+      <c r="A44" s="41"/>
       <c r="B44" s="17" t="s">
         <v>122</v>
       </c>
@@ -2145,7 +2145,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="47"/>
+      <c r="A45" s="42"/>
       <c r="B45" s="28" t="s">
         <v>123</v>
       </c>
@@ -2174,22 +2174,22 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="B46" s="44"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="40"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="39"/>
       <c r="I46" s="30"/>
       <c r="J46" s="30"/>
       <c r="K46" s="30"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="40" t="s">
         <v>126</v>
       </c>
       <c r="B47" s="17" t="s">
@@ -2222,7 +2222,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="46"/>
+      <c r="A48" s="41"/>
       <c r="B48" s="17" t="s">
         <v>131</v>
       </c>
@@ -2253,7 +2253,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="46"/>
+      <c r="A49" s="41"/>
       <c r="B49" s="33" t="s">
         <v>132</v>
       </c>
@@ -2286,7 +2286,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="46"/>
+      <c r="A50" s="41"/>
       <c r="B50" s="33" t="s">
         <v>133</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="46"/>
+      <c r="A51" s="41"/>
       <c r="B51" s="17" t="s">
         <v>134</v>
       </c>
@@ -2346,7 +2346,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="47"/>
+      <c r="A52" s="42"/>
       <c r="B52" s="28" t="s">
         <v>135</v>
       </c>
@@ -2375,22 +2375,22 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="43" t="s">
+      <c r="A53" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="B53" s="44"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
-      <c r="H53" s="40"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="39"/>
       <c r="I53" s="30"/>
       <c r="J53" s="30"/>
       <c r="K53" s="30"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="45" t="s">
+      <c r="A54" s="40" t="s">
         <v>138</v>
       </c>
       <c r="B54" s="17" t="s">
@@ -2425,7 +2425,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="46"/>
+      <c r="A55" s="41"/>
       <c r="B55" s="17" t="s">
         <v>142</v>
       </c>
@@ -2458,7 +2458,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="46"/>
+      <c r="A56" s="41"/>
       <c r="B56" s="17" t="s">
         <v>143</v>
       </c>
@@ -2487,7 +2487,7 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="47"/>
+      <c r="A57" s="42"/>
       <c r="B57" s="17" t="s">
         <v>144</v>
       </c>
@@ -2516,16 +2516,16 @@
       </c>
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="43" t="s">
+      <c r="A58" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="B58" s="44"/>
-      <c r="C58" s="44"/>
-      <c r="D58" s="44"/>
-      <c r="E58" s="44"/>
-      <c r="F58" s="44"/>
-      <c r="G58" s="44"/>
-      <c r="H58" s="40"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="38"/>
+      <c r="H58" s="39"/>
       <c r="I58" s="30"/>
       <c r="J58" s="30"/>
       <c r="K58" s="30"/>
@@ -3511,6 +3511,11 @@
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="A58:H58"/>
     <mergeCell ref="A47:A52"/>
     <mergeCell ref="A36:A45"/>
@@ -3523,11 +3528,6 @@
     <mergeCell ref="A35:H35"/>
     <mergeCell ref="A46:H46"/>
     <mergeCell ref="A53:H53"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F14 F15:G15 F16:F28 F29:H30 F31 F32:H32 F33:F34 F36:F45 F47:G48 F49:H49 F50:G50 F51:F52 F54:H55 F56:F57" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>